<commit_message>
read from excel, create test modules and execute code
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/Fasb2.xlsx
+++ b/src/main/resources/modules/Fasb2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\testing\AMTDirect_NousAutomation\Framework\Modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\seleniumAmtTesting\src\main\resources\modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EA8ED0-BF92-41E5-9F7B-BA3250189901}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F674279-09C9-4915-8A37-BB35F89A2E48}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="162">
   <si>
     <t>UserName</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t xml:space="preserve">  Troubleshooting  Check Rental Activity &amp; Payment Schedule</t>
+  </si>
+  <si>
+    <t>UIText.SetText</t>
   </si>
 </sst>
 </file>
@@ -3572,19 +3575,9 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Controller"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="TC001_TC050"/>
-      <sheetName val="TC051_TC100"/>
-      <sheetName val="TC101_TC150"/>
-      <sheetName val="TC151_TC200"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4602,10 +4595,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4690,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>21</v>
@@ -4699,7 +4692,7 @@
         <v>44</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4714,7 +4707,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>22</v>
@@ -4726,7 +4719,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4741,7 +4734,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>23</v>
@@ -4750,7 +4743,7 @@
         <v>201483</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4797,7 +4790,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4817,7 +4810,7 @@
       <c r="F8" s="57"/>
       <c r="G8" s="71"/>
       <c r="I8" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4837,7 +4830,7 @@
       <c r="F9" s="57"/>
       <c r="G9" s="71"/>
       <c r="I9" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4859,7 +4852,7 @@
         <v>131</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4881,7 +4874,7 @@
       <c r="F11" s="29"/>
       <c r="G11" s="3"/>
       <c r="I11" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4903,7 +4896,7 @@
       <c r="F12" s="29"/>
       <c r="G12" s="3"/>
       <c r="I12" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4925,7 +4918,7 @@
       <c r="F13" s="29"/>
       <c r="G13" s="3"/>
       <c r="I13" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4949,7 +4942,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4973,7 +4966,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4998,7 +4991,7 @@
       <c r="G16" s="60"/>
       <c r="H16" s="42"/>
       <c r="I16" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5021,7 +5014,7 @@
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5048,7 +5041,7 @@
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5077,7 +5070,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -5101,7 +5094,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5126,7 +5119,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5153,7 +5146,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5180,7 +5173,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5205,7 +5198,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5232,7 +5225,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5257,7 +5250,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5282,7 +5275,7 @@
         <v>6</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -5307,7 +5300,7 @@
         <v>6</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.25">
@@ -5332,7 +5325,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5359,7 +5352,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5382,7 +5375,7 @@
       <c r="G31" s="44"/>
       <c r="H31" s="1"/>
       <c r="I31" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5405,7 +5398,7 @@
       </c>
       <c r="H32" s="61"/>
       <c r="I32" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5430,7 +5423,7 @@
       <c r="G33" s="60"/>
       <c r="H33" s="42"/>
       <c r="I33" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5453,7 +5446,7 @@
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5480,7 +5473,7 @@
       </c>
       <c r="H35" s="61"/>
       <c r="I35" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5505,7 +5498,7 @@
         <v>6</v>
       </c>
       <c r="I36" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5530,7 +5523,7 @@
       </c>
       <c r="H37" s="61"/>
       <c r="I37" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5553,7 +5546,7 @@
       <c r="G38" s="64"/>
       <c r="H38" s="61"/>
       <c r="I38" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5576,7 +5569,7 @@
       </c>
       <c r="H39" s="61"/>
       <c r="I39" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5601,7 +5594,7 @@
       </c>
       <c r="H40" s="61"/>
       <c r="I40" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5624,7 +5617,7 @@
       <c r="G41" s="64"/>
       <c r="H41" s="61"/>
       <c r="I41" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5647,7 +5640,7 @@
       </c>
       <c r="H42" s="61"/>
       <c r="I42" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5674,7 +5667,7 @@
       </c>
       <c r="H43" s="61"/>
       <c r="I43" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5701,7 +5694,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5726,7 +5719,7 @@
         <v>6</v>
       </c>
       <c r="I45" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -5755,7 +5748,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J46" s="65"/>
     </row>
@@ -5779,7 +5772,7 @@
       <c r="G47" s="64"/>
       <c r="H47" s="61"/>
       <c r="I47" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J47" s="65"/>
     </row>
@@ -5805,7 +5798,7 @@
       <c r="G48" s="60"/>
       <c r="H48" s="42"/>
       <c r="I48" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -5828,7 +5821,7 @@
       </c>
       <c r="H49" s="61"/>
       <c r="I49" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -5857,7 +5850,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J50"/>
     </row>
@@ -5883,7 +5876,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="J51"/>
     </row>
@@ -5913,7 +5906,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5938,7 +5931,7 @@
       <c r="G53" s="60"/>
       <c r="H53" s="42"/>
       <c r="I53" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -5961,7 +5954,7 @@
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -10184,7 +10177,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="157" operator="equal" id="{D9FFFD8D-1B30-4FFA-AABF-1704792A3073}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -10197,7 +10190,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="156" operator="equal" id="{EED0F56C-5FAE-43B8-94F7-55A304F806D8}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -10223,7 +10216,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="153" operator="equal" id="{B6B3414D-98F7-45CF-A71B-556A092E8F5A}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -10236,7 +10229,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="152" operator="equal" id="{14A83E40-37A9-4A95-8996-23800E2FB4E3}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -10425,7 +10418,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="95" operator="equal" id="{A1824B24-4A66-4EE8-A8A9-E2B90CAF0C9C}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -10438,7 +10431,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="94" operator="equal" id="{29ED2F50-E459-464A-A705-D63B2DCBC0DD}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -11035,7 +11028,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="2" operator="equal" id="{3E1024D8-6003-4F4C-8081-4741D4C3DE63}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -11048,7 +11041,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="1" operator="equal" id="{0E49373A-46A3-4BD9-8E95-5F72216F45AC}">
-            <xm:f>'E:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\nous_1172018\AMTDirect_NousAutomation\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>

</xml_diff>